<commit_message>
Small code changes and refinments
</commit_message>
<xml_diff>
--- a/data/output/seat_status_classroom_image12.xlsx
+++ b/data/output/seat_status_classroom_image12.xlsx
@@ -567,13 +567,13 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1125.814697265625</v>
+        <v>1125.814819335938</v>
       </c>
       <c r="B5" t="n">
-        <v>610.1145629882812</v>
+        <v>610.1146240234375</v>
       </c>
       <c r="C5" t="n">
-        <v>1200.769409179688</v>
+        <v>1200.769287109375</v>
       </c>
       <c r="D5" t="n">
         <v>657.3201904296875</v>
@@ -837,19 +837,19 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>84.45109558105469</v>
+        <v>84.45108032226562</v>
       </c>
       <c r="B14" t="n">
-        <v>616.6791381835938</v>
+        <v>616.6790771484375</v>
       </c>
       <c r="C14" t="n">
-        <v>206.3239593505859</v>
+        <v>206.3239898681641</v>
       </c>
       <c r="D14" t="n">
         <v>786.3602294921875</v>
       </c>
       <c r="E14" t="n">
-        <v>145.3875274658203</v>
+        <v>145.3875427246094</v>
       </c>
       <c r="F14" t="n">
         <v>701.5196533203125</v>
@@ -897,7 +897,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1556.228515625</v>
+        <v>1556.228637695312</v>
       </c>
       <c r="B16" t="n">
         <v>706.8097534179688</v>
@@ -990,19 +990,19 @@
         <v>115.7835540771484</v>
       </c>
       <c r="B19" t="n">
-        <v>677.7320556640625</v>
+        <v>677.732177734375</v>
       </c>
       <c r="C19" t="n">
         <v>278.8323974609375</v>
       </c>
       <c r="D19" t="n">
-        <v>850.528076171875</v>
+        <v>850.5281982421875</v>
       </c>
       <c r="E19" t="n">
         <v>197.3079833984375</v>
       </c>
       <c r="F19" t="n">
-        <v>764.1300659179688</v>
+        <v>764.1301879882812</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1017,13 +1017,13 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>832.919921875</v>
+        <v>832.9198608398438</v>
       </c>
       <c r="B20" t="n">
         <v>735.2488403320312</v>
       </c>
       <c r="C20" t="n">
-        <v>880.513916015625</v>
+        <v>880.5139770507812</v>
       </c>
       <c r="D20" t="n">
         <v>819.7266845703125</v>
@@ -1047,22 +1047,22 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1132.585693359375</v>
+        <v>1132.585815429688</v>
       </c>
       <c r="B21" t="n">
-        <v>741.4110717773438</v>
+        <v>741.4111328125</v>
       </c>
       <c r="C21" t="n">
-        <v>1294.633056640625</v>
+        <v>1294.633178710938</v>
       </c>
       <c r="D21" t="n">
-        <v>827.8931274414062</v>
+        <v>827.8931884765625</v>
       </c>
       <c r="E21" t="n">
-        <v>1213.609375</v>
+        <v>1213.609497070312</v>
       </c>
       <c r="F21" t="n">
-        <v>784.652099609375</v>
+        <v>784.6521606445312</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1140,19 +1140,19 @@
         <v>866.8123779296875</v>
       </c>
       <c r="B24" t="n">
-        <v>760.72412109375</v>
+        <v>760.7243041992188</v>
       </c>
       <c r="C24" t="n">
         <v>1083.017333984375</v>
       </c>
       <c r="D24" t="n">
-        <v>1066.103271484375</v>
+        <v>1066.103393554688</v>
       </c>
       <c r="E24" t="n">
         <v>974.9148559570312</v>
       </c>
       <c r="F24" t="n">
-        <v>913.4136962890625</v>
+        <v>913.413818359375</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>

</xml_diff>